<commit_message>
fixed LCD contrast resistors
</commit_message>
<xml_diff>
--- a/rev_b/hdw/Pulse_Oximeter/Pulse_Oximeter_bom_B.xlsx
+++ b/rev_b/hdw/Pulse_Oximeter/Pulse_Oximeter_bom_B.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\pulse_oximeter\hdw\rev_b\Pulse_Oximeter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\pulse_oximeter\rev_b\hdw\Pulse_Oximeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638538F3-9DBA-4438-AA2F-842207FCF79C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA38FF2-7489-4169-815C-3906905A791E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,9 +280,6 @@
     <t>RMCF0402FT27R0CT-ND</t>
   </si>
   <si>
-    <t>R407 R603 R604 R801 R803 R1003 R1603</t>
-  </si>
-  <si>
     <t>RMCF0402FT100RCT-ND</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>RMCF0402FT6K04CT-ND</t>
   </si>
   <si>
-    <t>R202 R205 R206 R212 R214 R218 R219 R220 R401 R403 R404 R405 R406 R601 R602 R802 R804 R1001 R1004 R1101 R1102 R1501 R1502 R1505 R1506 R1507 R1601 R1602 R1604 R1605 R1606 R1607 R1609 R1610 R1611 R1612 R1613 R1614 R1615 R1703 R1704 R1705 R1801 R1901 R1902 R1905 R1906 R2001 R2003</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -554,6 +548,12 @@
   </si>
   <si>
     <t>535-9558-1-ND</t>
+  </si>
+  <si>
+    <t>R407 R603 R604 R801 R803 R1003 R1604</t>
+  </si>
+  <si>
+    <t>R202 R205 R206 R212 R214 R218 R219 R220 R401 R403 R404 R405 R406 R601 R602 R802 R804 R1001 R1004 R1101 R1102 R1501 R1502 R1505 R1506 R1507 R1601 R1602 R1603 R1605 R1606 R1607 R1609 R1610 R1611 R1612 R1613 R1614 R1615 R1703 R1704 R1705 R1801 R1901 R1902 R1905 R1906 R2001 R2003</t>
   </si>
 </sst>
 </file>
@@ -1403,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="B37" s="1">
         <v>100</v>
@@ -2003,22 +2003,22 @@
         <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>8</v>
@@ -2026,31 +2026,31 @@
     </row>
     <row r="39" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1">
         <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>8</v>
@@ -2058,31 +2058,31 @@
     </row>
     <row r="41" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C41" s="1">
         <v>49</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>21</v>
@@ -2090,16 +2090,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>8</v>
@@ -2107,16 +2107,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>8</v>
@@ -2124,31 +2124,31 @@
     </row>
     <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C45" s="1">
         <v>6</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>21</v>
@@ -2156,16 +2156,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>8</v>
@@ -2173,16 +2173,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>21</v>
@@ -2190,10 +2190,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
@@ -2203,10 +2203,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
@@ -2216,91 +2216,91 @@
     </row>
     <row r="51" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C51" s="1">
         <v>5</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C52" s="1">
         <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C53" s="1">
         <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>19</v>
@@ -2308,16 +2308,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C57" s="1">
-        <v>1</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>8</v>
@@ -2325,10 +2325,10 @@
     </row>
     <row r="58" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
@@ -2338,16 +2338,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C59" s="1">
         <v>4</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>17</v>
@@ -2355,16 +2355,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>21</v>
@@ -2372,31 +2372,31 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C62" s="1">
         <v>5</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>17</v>
@@ -2404,31 +2404,31 @@
     </row>
     <row r="63" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>21</v>
@@ -2436,16 +2436,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>8</v>
@@ -2453,16 +2453,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C66" s="1">
-        <v>1</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>8</v>
@@ -2470,91 +2470,91 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="C67" s="1">
-        <v>1</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C69" s="1">
-        <v>1</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="C71" s="1">
-        <v>1</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C72" s="1">
-        <v>1</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>21</v>

</xml_diff>